<commit_message>
Fix notification enable and disable.
</commit_message>
<xml_diff>
--- a/Change Track.xlsx
+++ b/Change Track.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Change Number</t>
   </si>
@@ -37,6 +37,12 @@
   </si>
   <si>
     <t>01</t>
+  </si>
+  <si>
+    <t>Done</t>
+  </si>
+  <si>
+    <t>Status</t>
   </si>
 </sst>
 </file>
@@ -386,20 +392,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="15.28515625" style="1" customWidth="1"/>
     <col min="2" max="2" width="8.42578125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="94.42578125" customWidth="1"/>
+    <col min="4" max="4" width="75.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="30">
+    <row r="1" spans="1:5" ht="30">
       <c r="A1" s="3" t="s">
         <v>2</v>
       </c>
@@ -412,8 +418,11 @@
       <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
+      <c r="E1" t="s">
+        <v>8</v>
+      </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:5">
       <c r="A2" s="5">
         <v>41681</v>
       </c>
@@ -425,6 +434,9 @@
       </c>
       <c r="D2" t="s">
         <v>5</v>
+      </c>
+      <c r="E2" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
OS Task Initial Release
</commit_message>
<xml_diff>
--- a/Change Track.xlsx
+++ b/Change Track.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="15">
   <si>
     <t>Change Number</t>
   </si>
@@ -43,6 +43,24 @@
   </si>
   <si>
     <t>Status</t>
+  </si>
+  <si>
+    <t>JMR</t>
+  </si>
+  <si>
+    <t>OS Tick Initial Release</t>
+  </si>
+  <si>
+    <t>00</t>
+  </si>
+  <si>
+    <t>02</t>
+  </si>
+  <si>
+    <t>OS Task Initial Release</t>
+  </si>
+  <si>
+    <t>On Process</t>
   </si>
 </sst>
 </file>
@@ -78,7 +96,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -97,6 +115,9 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -392,16 +413,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="15.28515625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="8.42578125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="8.42578125" style="6" customWidth="1"/>
+    <col min="3" max="3" width="11.42578125" style="1"/>
     <col min="4" max="4" width="75.7109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -409,7 +431,7 @@
       <c r="A1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="7" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="4" t="s">
@@ -427,16 +449,50 @@
         <v>41681</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D2" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="E2" t="s">
         <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="5">
+        <v>41681</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="5">
+        <v>41699</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adding PIT changes track
</commit_message>
<xml_diff>
--- a/Change Track.xlsx
+++ b/Change Track.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="105" windowWidth="15120" windowHeight="8010"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="17">
   <si>
     <t>Change Number</t>
   </si>
@@ -61,13 +61,19 @@
   </si>
   <si>
     <t>On Process</t>
+  </si>
+  <si>
+    <t>03</t>
+  </si>
+  <si>
+    <t>Update from GPT naming to PIT</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -125,11 +131,16 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -203,6 +214,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -237,6 +249,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -412,14 +425,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.28515625" style="1" customWidth="1"/>
     <col min="2" max="2" width="8.42578125" style="6" customWidth="1"/>
@@ -427,7 +440,7 @@
     <col min="4" max="4" width="75.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="30">
+    <row r="1" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>2</v>
       </c>
@@ -444,7 +457,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="5">
         <v>41681</v>
       </c>
@@ -461,7 +474,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="5">
         <v>41681</v>
       </c>
@@ -478,7 +491,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
         <v>41699</v>
       </c>
@@ -493,6 +506,23 @@
       </c>
       <c r="E4" t="s">
         <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="5">
+        <v>41699</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -502,12 +532,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -515,12 +545,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>

</xml_diff>

<commit_message>
Report documents for Scheduler updated
</commit_message>
<xml_diff>
--- a/Change Track.xlsx
+++ b/Change Track.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="105" windowWidth="15120" windowHeight="8010"/>
@@ -11,12 +11,12 @@
     <sheet name="Tabelle2" sheetId="2" r:id="rId2"/>
     <sheet name="Tabelle3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="26">
   <si>
     <t>Change Number</t>
   </si>
@@ -67,13 +67,40 @@
   </si>
   <si>
     <t>Update from GPT naming to PIT</t>
+  </si>
+  <si>
+    <t>04</t>
+  </si>
+  <si>
+    <t>JEB</t>
+  </si>
+  <si>
+    <t>System Design document updated</t>
+  </si>
+  <si>
+    <t>05</t>
+  </si>
+  <si>
+    <t>Test Cases Document for Scheduler Updated</t>
+  </si>
+  <si>
+    <t>06</t>
+  </si>
+  <si>
+    <t>Traceability document for Scheduler Updated</t>
+  </si>
+  <si>
+    <t>07</t>
+  </si>
+  <si>
+    <t>Report Documents updated</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -214,7 +241,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -249,7 +275,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -425,14 +450,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="15.28515625" style="1" customWidth="1"/>
     <col min="2" max="2" width="8.42578125" style="6" customWidth="1"/>
@@ -440,7 +465,7 @@
     <col min="4" max="4" width="75.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="30">
       <c r="A1" s="3" t="s">
         <v>2</v>
       </c>
@@ -457,7 +482,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5">
       <c r="A2" s="5">
         <v>41681</v>
       </c>
@@ -474,7 +499,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5">
       <c r="A3" s="5">
         <v>41681</v>
       </c>
@@ -491,7 +516,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5">
       <c r="A4" s="5">
         <v>41699</v>
       </c>
@@ -508,7 +533,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5">
       <c r="A5" s="5">
         <v>41699</v>
       </c>
@@ -522,6 +547,74 @@
         <v>16</v>
       </c>
       <c r="E5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="5">
+        <v>41710</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="5">
+        <v>41710</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" t="s">
+        <v>21</v>
+      </c>
+      <c r="E7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" s="5">
+        <v>41710</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D8" t="s">
+        <v>23</v>
+      </c>
+      <c r="E8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" s="5">
+        <v>41711</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" t="s">
+        <v>25</v>
+      </c>
+      <c r="E9" t="s">
         <v>7</v>
       </c>
     </row>
@@ -532,12 +625,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -545,12 +638,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>

</xml_diff>

<commit_message>
Initial updates for Homework 3
</commit_message>
<xml_diff>
--- a/Change Track.xlsx
+++ b/Change Track.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="30">
   <si>
     <t>Change Number</t>
   </si>
@@ -94,6 +94,18 @@
   </si>
   <si>
     <t>Report Documents updated</t>
+  </si>
+  <si>
+    <t>08</t>
+  </si>
+  <si>
+    <t>Initial Requirements matrix for Homework 3</t>
+  </si>
+  <si>
+    <t>09</t>
+  </si>
+  <si>
+    <t>Project folder for homework 3</t>
   </si>
 </sst>
 </file>
@@ -451,10 +463,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -615,6 +627,40 @@
         <v>25</v>
       </c>
       <c r="E9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" s="5">
+        <v>41720</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D10" t="s">
+        <v>27</v>
+      </c>
+      <c r="E10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" s="5">
+        <v>41720</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D11" t="s">
+        <v>29</v>
+      </c>
+      <c r="E11" t="s">
         <v>7</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Review Change Track and update accordantly.
</commit_message>
<xml_diff>
--- a/Change Track.xlsx
+++ b/Change Track.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="105" windowWidth="15120" windowHeight="8010"/>
@@ -11,12 +11,12 @@
     <sheet name="Tabelle2" sheetId="2" r:id="rId2"/>
     <sheet name="Tabelle3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="29">
   <si>
     <t>Change Number</t>
   </si>
@@ -58,9 +58,6 @@
   </si>
   <si>
     <t>OS Task Initial Release</t>
-  </si>
-  <si>
-    <t>On Process</t>
   </si>
   <si>
     <t>03</t>
@@ -179,7 +176,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -466,10 +463,10 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="G5" sqref="G4:G5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="15.28515625" style="1" customWidth="1"/>
     <col min="2" max="2" width="8.42578125" style="6" customWidth="1"/>
@@ -542,7 +539,7 @@
         <v>13</v>
       </c>
       <c r="E4" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -550,13 +547,13 @@
         <v>41699</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>9</v>
       </c>
       <c r="D5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E5" t="s">
         <v>7</v>
@@ -567,13 +564,13 @@
         <v>41710</v>
       </c>
       <c r="B6" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="D6" t="s">
         <v>18</v>
-      </c>
-      <c r="D6" t="s">
-        <v>19</v>
       </c>
       <c r="E6" t="s">
         <v>7</v>
@@ -584,13 +581,13 @@
         <v>41710</v>
       </c>
       <c r="B7" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" t="s">
         <v>20</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D7" t="s">
-        <v>21</v>
       </c>
       <c r="E7" t="s">
         <v>7</v>
@@ -601,13 +598,13 @@
         <v>41710</v>
       </c>
       <c r="B8" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" t="s">
         <v>22</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D8" t="s">
-        <v>23</v>
       </c>
       <c r="E8" t="s">
         <v>7</v>
@@ -618,13 +615,13 @@
         <v>41711</v>
       </c>
       <c r="B9" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D9" t="s">
         <v>24</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D9" t="s">
-        <v>25</v>
       </c>
       <c r="E9" t="s">
         <v>7</v>
@@ -635,13 +632,13 @@
         <v>41720</v>
       </c>
       <c r="B10" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D10" t="s">
         <v>26</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D10" t="s">
-        <v>27</v>
       </c>
       <c r="E10" t="s">
         <v>7</v>
@@ -652,13 +649,13 @@
         <v>41720</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>9</v>
       </c>
       <c r="D11" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E11" t="s">
         <v>7</v>
@@ -676,7 +673,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -689,7 +686,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>

</xml_diff>

<commit_message>
OS Dispatcher and OSEK functions
</commit_message>
<xml_diff>
--- a/Change Track.xlsx
+++ b/Change Track.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="32">
   <si>
     <t>Change Number</t>
   </si>
@@ -103,6 +103,15 @@
   </si>
   <si>
     <t>Project folder for homework 3</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>OS Dispatcher and OSEK functions</t>
+  </si>
+  <si>
+    <t>In process</t>
   </si>
 </sst>
 </file>
@@ -460,10 +469,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G4:G5"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -659,6 +668,23 @@
       </c>
       <c r="E11" t="s">
         <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" s="5">
+        <v>41727</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D12" t="s">
+        <v>30</v>
+      </c>
+      <c r="E12" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update for initial Project Name Practice 4
</commit_message>
<xml_diff>
--- a/Change Track.xlsx
+++ b/Change Track.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="105" windowWidth="15120" windowHeight="8010"/>
@@ -11,12 +11,12 @@
     <sheet name="Tabelle2" sheetId="2" r:id="rId2"/>
     <sheet name="Tabelle3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="34">
   <si>
     <t>Change Number</t>
   </si>
@@ -112,6 +112,12 @@
   </si>
   <si>
     <t>In process</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Initial Base Project </t>
   </si>
 </sst>
 </file>
@@ -185,7 +191,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -469,13 +475,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="15.28515625" style="1" customWidth="1"/>
     <col min="2" max="2" width="8.42578125" style="6" customWidth="1"/>
@@ -685,6 +691,23 @@
       </c>
       <c r="E12" t="s">
         <v>31</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" s="5">
+        <v>41755</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D13" t="s">
+        <v>33</v>
+      </c>
+      <c r="E13" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -699,7 +722,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -712,7 +735,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>

</xml_diff>

<commit_message>
Additional comment included due to traceability matrix
</commit_message>
<xml_diff>
--- a/Change Track.xlsx
+++ b/Change Track.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="36">
   <si>
     <t>Change Number</t>
   </si>
@@ -118,6 +118,12 @@
   </si>
   <si>
     <t xml:space="preserve">Initial Base Project </t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>Initial responsibilities asigned in requirements document</t>
   </si>
 </sst>
 </file>
@@ -475,10 +481,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -707,6 +713,23 @@
         <v>33</v>
       </c>
       <c r="E13" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" s="5">
+        <v>41755</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D14" t="s">
+        <v>35</v>
+      </c>
+      <c r="E14" t="s">
         <v>7</v>
       </c>
     </row>

</xml_diff>